<commit_message>
Reports destinations changed to same directory
</commit_message>
<xml_diff>
--- a/CarDealersSystem/CarDealersSystem.ConsoleClient/bin/Debug/Report.xlsx
+++ b/CarDealersSystem/CarDealersSystem.ConsoleClient/bin/Debug/Report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Bugs" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="14">
   <si>
     <t>CarModel</t>
   </si>
@@ -34,6 +34,30 @@
   </si>
   <si>
     <t>TotalIncome</t>
+  </si>
+  <si>
+    <t>Astra</t>
+  </si>
+  <si>
+    <t>Opel</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>621000</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>690000</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>713000</t>
   </si>
 </sst>
 </file>
@@ -73,7 +97,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -81,14 +105,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office тема">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Оffice">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -126,9 +153,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Оffice">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -163,7 +190,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -198,7 +225,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Оffice">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -371,11 +398,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="C4" sqref="A2:C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,7 +412,7 @@
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row spans="1:3" x14ac:dyDescent="0.25" outlineLevel="0" r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -394,159 +421,6 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="2">
-      <c r="A2" s="0" t="inlineStr">
-        <is>
-          <t>Opel Astra</t>
-        </is>
-      </c>
-      <c r="B2" s="0" t="inlineStr">
-        <is>
-          <t>Break fluid leak</t>
-        </is>
-      </c>
-      <c r="C2" s="0" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="3">
-      <c r="A3" s="0" t="inlineStr">
-        <is>
-          <t>Opel Corsa</t>
-        </is>
-      </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>Engine problem</t>
-        </is>
-      </c>
-      <c r="C3" s="0" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="4">
-      <c r="A4" s="0" t="inlineStr">
-        <is>
-          <t>Mitsubishi Space Star</t>
-        </is>
-      </c>
-      <c r="B4" s="0" t="inlineStr">
-        <is>
-          <t>Thick-Thick Steering Wheel Sounds</t>
-        </is>
-      </c>
-      <c r="C4" s="0" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="5">
-      <c r="A5" s="0" t="inlineStr">
-        <is>
-          <t>Opel Astra</t>
-        </is>
-      </c>
-      <c r="B5" s="0" t="inlineStr">
-        <is>
-          <t>Break fluid leak</t>
-        </is>
-      </c>
-      <c r="C5" s="0" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="6">
-      <c r="A6" s="0" t="inlineStr">
-        <is>
-          <t>Opel Corsa</t>
-        </is>
-      </c>
-      <c r="B6" s="0" t="inlineStr">
-        <is>
-          <t>Engine problem</t>
-        </is>
-      </c>
-      <c r="C6" s="0" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="7">
-      <c r="A7" s="0" t="inlineStr">
-        <is>
-          <t>Mitsubishi Space Star</t>
-        </is>
-      </c>
-      <c r="B7" s="0" t="inlineStr">
-        <is>
-          <t>Thick-Thick Steering Wheel Sounds</t>
-        </is>
-      </c>
-      <c r="C7" s="0" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="8">
-      <c r="A8" s="0" t="inlineStr">
-        <is>
-          <t>Opel Astra</t>
-        </is>
-      </c>
-      <c r="B8" s="0" t="inlineStr">
-        <is>
-          <t>Break fluid leak</t>
-        </is>
-      </c>
-      <c r="C8" s="0" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="9">
-      <c r="A9" s="0" t="inlineStr">
-        <is>
-          <t>Opel Corsa</t>
-        </is>
-      </c>
-      <c r="B9" s="0" t="inlineStr">
-        <is>
-          <t>Engine problem</t>
-        </is>
-      </c>
-      <c r="C9" s="0" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="10">
-      <c r="A10" s="0" t="inlineStr">
-        <is>
-          <t>Mitsubishi Space Star</t>
-        </is>
-      </c>
-      <c r="B10" s="0" t="inlineStr">
-        <is>
-          <t>Thick-Thick Steering Wheel Sounds</t>
-        </is>
-      </c>
-      <c r="C10" s="0" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
       </c>
     </row>
   </sheetData>
@@ -556,7 +430,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -584,6 +458,132 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>